<commit_message>
add testcase for RuleManager
</commit_message>
<xml_diff>
--- a/doc/TestCase_0616.xlsx
+++ b/doc/TestCase_0616.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16128" windowHeight="7488"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Test" sheetId="1" r:id="rId1"/>
     <sheet name="Integration Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,11 +101,6 @@
   </si>
   <si>
     <t>TC ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Expected
-Output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -154,14 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Send Action command event to NodeManager  via EventBus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NodeManager receives Action event</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC_NM_002</t>
   </si>
   <si>
@@ -269,10 +256,6 @@
   </si>
   <si>
     <t>TC_RM_002</t>
-  </si>
-  <si>
-    <t>makeRule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TC_SA_001</t>
@@ -343,13 +326,142 @@
   </si>
   <si>
     <t>send JSON message of Sensor status  to WiFi</t>
+  </si>
+  <si>
+    <t>createRule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create a rule (do actions in condition) 
+1. Check validity with exist rule in ruleset. (same rule, and conflict rule)
+2. Return false if new rule is not valid on 1. 
+3. If it is new rule, create rule.
+4. If there are ruls on same condition, add new actions on exist rule. 
+5. Update ruleset based on 3~4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">T/F  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A or nodeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Search rules on specified condition and return matched rule.
+2. Return whole rules if condition does not specified.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchRule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleteRule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rule := Actions + Conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rule statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rule statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">T/F  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Search rule on givin condition. 
+2. delete actions if there are some actions left on same condition.
+3. delete rule if there is no action left on same condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode (alarm, normal)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Do actions if exist based on rule.      (ex. Close door before set alarm)
+2. cancle sheduled actions if exist.        (ex. If alarm unset, delete scheduled alarm set action)
+3. activate/deactivate rules based on the mode. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>action statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. send rules to UI via EventBus. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Search action list on current condition (mode)
+2. check action is on not allowed list.       (ex. Do not open in alarm mode)
+3. execute action if it is not blocked on rule.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. send actions event to NodeManager via EventBus
+2. Ignore actions if it is prohivited with rule </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do_thingEvent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -435,13 +547,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,6 +605,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,38 +890,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H23"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="1" customWidth="1"/>
     <col min="8" max="8" width="21.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.09765625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="53.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="53.375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -785,7 +937,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="34.799999999999997">
+    <row r="2" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -802,10 +954,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
@@ -814,13 +966,13 @@
         <v>7</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="52.2">
+    <row r="3" spans="1:12" ht="132" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -831,25 +983,31 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12">
+        <v>22</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -858,286 +1016,368 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12">
+        <v>22</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="K5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="K6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="34.799999999999997">
-      <c r="B11" s="3" t="s">
+    <row r="10" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="34.799999999999997">
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="34.799999999999997">
+    <row r="13" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="34.799999999999997">
+    <row r="14" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="34.799999999999997">
+    <row r="15" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="52.2">
+    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="2:12" ht="34.799999999999997">
+    <row r="17" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1150,7 +1390,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1163,123 +1403,123 @@
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="2:12" ht="34.799999999999997">
+    <row r="20" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="2:12" ht="34.799999999999997">
-      <c r="B21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="2:12" ht="34.799999999999997">
+    <row r="22" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="2:12" ht="34.799999999999997">
+    <row r="23" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1292,7 +1532,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1305,18 +1545,18 @@
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1326,7 +1566,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1339,7 +1579,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1352,7 +1592,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1365,7 +1605,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1378,7 +1618,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1391,7 +1631,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1404,7 +1644,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1417,7 +1657,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1430,7 +1670,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1443,7 +1683,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1456,7 +1696,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1469,7 +1709,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1482,7 +1722,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1495,7 +1735,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1508,7 +1748,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1521,7 +1761,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1534,7 +1774,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1547,7 +1787,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="2:12">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1560,7 +1800,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="2:12">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1573,7 +1813,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1586,7 +1826,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1599,7 +1839,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1612,7 +1852,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -1625,7 +1865,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="2:12">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -1638,7 +1878,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="2:12">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -1651,7 +1891,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -1664,7 +1904,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="2:12">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -1677,7 +1917,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="2:12">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -1690,7 +1930,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1703,7 +1943,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -1716,7 +1956,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -1729,7 +1969,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -1742,7 +1982,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -1755,7 +1995,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="2:12">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -1768,7 +2008,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="2:12">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1781,7 +2021,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="2:12">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -1794,7 +2034,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="2:12">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -1807,7 +2047,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="2:12">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -1820,7 +2060,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -1833,7 +2073,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -1846,7 +2086,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="2:12">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -1859,7 +2099,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1872,7 +2112,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="2:12">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1885,7 +2125,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="2:12">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -1898,7 +2138,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="2:12">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -1911,7 +2151,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="2:12">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -1924,7 +2164,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="2:12">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -1937,7 +2177,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="2:12">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -1950,7 +2190,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="2:12">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -1963,7 +2203,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="2:12">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1976,7 +2216,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="2:12">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1989,7 +2229,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="2:12">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -2002,7 +2242,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -2027,12 +2267,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update RuleManager test case
</commit_message>
<xml_diff>
--- a/doc/TestCase_0616.xlsx
+++ b/doc/TestCase_0616.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -329,10 +329,6 @@
   </si>
   <si>
     <t>createRule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -454,6 +450,96 @@
   </si>
   <si>
     <t>changeConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actuator change evenet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. If the thing event is defined on ruleset, then send actions event to NodeManager via EventBus
+2. Do nothing if there is no rule on the even.t  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Search ruleset if the thing event matches conditions.
+2. If matches, execute actions.
+3. If matched actions is delay actions, put it to scheduler (such as turn off light after 10 mins)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thing event</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Get config value from UI.
+2. Update config value to DB.
+3. update delay time on delay action.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node connection info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateNode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. If node is disconnected, inactivate rules on the node.
+2. If node is connected, activate rules on the node. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_RM_008</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -603,9 +689,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -617,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,7 +976,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -900,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -922,20 +1008,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
@@ -957,7 +1043,7 @@
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
@@ -986,23 +1072,25 @@
         <v>71</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
@@ -1016,28 +1104,32 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1045,30 +1137,34 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1076,30 +1172,34 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1110,25 +1210,31 @@
         <v>13</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1136,20 +1242,34 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
+      <c r="L8" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1157,63 +1277,91 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="L9" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10" t="s">
+      <c r="E10" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="11"/>
+      <c r="L10" s="10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8" t="s">
+      <c r="I11" s="8"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="9"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">

</xml_diff>

<commit_message>
Testcase is updated - RuleManager
</commit_message>
<xml_diff>
--- a/doc/TestCase_0616.xlsx
+++ b/doc/TestCase_0616.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="116">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,10 +337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">T/F  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N/A or nodeID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -359,26 +355,6 @@
   </si>
   <si>
     <t>Rule := Actions + Conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rules</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rule statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rule statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">T/F  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rules</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -388,14 +364,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mode (alarm, normal)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>changeMode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -410,22 +378,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>action statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. send rules to UI via EventBus. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. Search action list on current condition (mode)
 2. check action is on not allowed list.       (ex. Do not open in alarm mode)
 3. execute action if it is not blocked on rule.</t>
@@ -449,10 +401,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Actuator change evenet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">1. If the thing event is defined on ruleset, then send actions event to NodeManager via EventBus
 2. Do nothing if there is no rule on the even.t  </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,27 +412,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>actions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thing event</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>configuration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>config time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -514,15 +442,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Node connection info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>updateNode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>node ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -540,6 +460,75 @@
   </si>
   <si>
     <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode (alarm, normal)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rule string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>action string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actuator change event</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thing string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node connection information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node ID, "
+Conn" / "DisConn"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Rule is added if no conflict
+2. Return error if conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. send searched rules to UI via EventBus. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Rule is deleted if exist.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. mode changed.
+2. rule is activate/inactivated based on mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. configuration value is changed .
+2. DB is updated.
+3. Delay action is updated. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. activate/inactivate rule on the node</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -976,7 +965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -986,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1043,10 +1032,10 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -1072,19 +1061,19 @@
         <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>21</v>
@@ -1104,31 +1093,33 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -1137,33 +1128,33 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -1172,33 +1163,33 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -1210,30 +1201,30 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -1242,33 +1233,33 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -1277,33 +1268,33 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
@@ -1312,28 +1303,28 @@
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="I10" s="10" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Test case 아두이노 부분 update
</commit_message>
<xml_diff>
--- a/doc/TestCase_0616.xlsx
+++ b/doc/TestCase_0616.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16128" windowHeight="7488"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Test" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,10 +267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SendJSONstatusEvent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC_SA_002</t>
   </si>
   <si>
@@ -292,36 +288,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>discover JSON message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>registered JSON message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sensor current value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> key , value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send JSON object to WiFi</t>
-  </si>
-  <si>
-    <t>send discover JSON message  to WiFi</t>
-  </si>
-  <si>
-    <t>send registered JSON message  to WiFi</t>
-  </si>
-  <si>
-    <t>send JSON message of Sensor status  to WiFi</t>
   </si>
   <si>
     <t>createRule</t>
@@ -531,12 +499,244 @@
     <t>1. activate/inactivate rule on the node</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">Job = "Discovered"
+NodeID = "12:23:34:45:56:67"
+ThingList =
+"0001","Door"       ,"Actuator","String","Open"  ,"Close"
+"0002","Light"      ,"Actuator","String","On"    ,"Off"  
+"0003","Presence"   ,"Sensor"  ,"String","AtHome","Away" 
+"0004","Temperature","Sensor"  ,"Number","-50"   ,"50"   
+"0005","Humidity"   ,"Sensor"  ,"Number","0"     ,"100" 
+"0006","DoorSensor" ,"Sensor"  ,"String","Open"  ,"Close"
+"0007","MailBox"    ,"Sensor"  ,"String","Empty" ,"Mail" 
+"0008","Alarm"      ,"Actuator","String","Set"   ,"Unset"
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Job = "Registered"
+NodeID = "12:23:34:45:56:67"
+Result = "Authorized"
+ThingList =
+"0001","Door"       ,"Actuator","String","Open"  ,"Close"
+"0002","Light"      ,"Actuator","String","On"    ,"Off"  
+"0003","Presence"   ,"Sensor"  ,"String","AtHome","Away" 
+"0004","Temperature","Sensor"  ,"Number","-50"   ,"50"   
+"0005","Humidity"   ,"Sensor"  ,"Number","0"     ,"100" 
+"0006","DoorSensor" ,"Sensor"  ,"String","Open"  ,"Close"
+"0007","MailBox"    ,"Sensor"  ,"String","Empty" ,"Mail" 
+"0008","Alarm"      ,"Actuator","String","Set"   ,"Unset"
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Job = "Registered"
+NodeID = "12:23:34:45:56:67"
+Status =
+"0003","Presence"   ,"Away" 
+"0004","Temperature","-999" 
+"0005","Humidity"   ,"100"  
+"0006","DoorSensor" ,"Close"
+"0007","MailBox"    ,"Mail"  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>registered JSON message
+- Job
+- NodeID
+- Result
+- ThingList : ID,Type, Stype, Vtype,Vmin, VMax</t>
+  </si>
+  <si>
+    <t>JSON object : key , value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"NodeID" , "12:23:34:45:56:67"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Send JSON object(below) to WiFi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"NodeID":"12:23:34:45:56:67"</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SendJSONstatusEvent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>discover JSON message
+- Job
+- NodeID
+- ThingList : ID,Type, Stype, Vtype,Vmin, VMax</t>
+  </si>
+  <si>
+    <t>1. Generate JSON object with key and value.
+2. Convert JSON obect to String
+3. Send String to WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Generate JSON message using things information
+2. Convert JSON message to String
+3. Send String to WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Generate JSON message using current sensor value
+2. Convert JSON message to String
+3. Send String to WiFi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>current sensor value JSON message
+- Job
+- NodeID
+- Status : ID,Type, Value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Send current sensor value JSON message(below) to WiFi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+"Job" : "Registered",
+"NodeID" : "12:23:34:45:56:67",
+"Status" : [
+{"Id":"0003","Type":"Presence"   ,"Value":"Away"}, 
+{"Id":"0004","Type":"Temperature","Value":"-999"}, 
+{"Id":"0005","Type":"Humidity"   ,"Value":"100"},  
+{"Id":"0006","Type":"DoorSensor" ,"Value":"Close"},
+{"Id":"0007","Type":"MailBox"    ,"Value":"Mail"}  
+]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Send discover JSON message(below) to WiFi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+"Job" : "Discovered",
+"NodeID" : "12:23:34:45:56:67",
+"ThingList" : [
+{"Id":"0001","Type":"Door"       ,"SType":"Actuator","VType": "String","VMin" : "Open"  ,"VMax" : "Close"},
+{"Id":"0002","Type":"Light"      ,"SType":"Actuator","VType": "String","VMin" : "On"    ,"VMax" : "Off"  },
+{"Id":"0003","Type":"Presence"   ,"SType":"Sensor"  ,"VType": "String","VMin" : "AtHome","VMax" : "Away" },
+{"Id":"0004","Type":"Temperature","SType":"Sensor"  ,"VType": "Number","VMin" : "-50"   ,"VMax" : "50"   },
+{"Id":"0005","Type":"Humidity"   ,"SType":"Sensor"  ,"VType": "Number","VMin" : "0"     ,"VMax" : "100" },
+{"Id":"0006","Type":"DoorSensor" ,"SType":"Sensor"  ,"VType": "String","VMin" : "Open"  ,"VMax" : "Close"},
+{"Id":"0007","Type":"MailBox"    ,"SType":"Sensor"  ,"VType": "String","VMin" : "Empty" ,"VMax" : "Mail" },
+{"Id":"0008","Type":"Alarm"      ,"SType":"Actuator","VType": "String","VMin" : "Set"   ,"VMax" : "Unset"}
+]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Send registered JSON message(below) to WiFi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+"Job" : "Registered",
+"NodeID" : "12:23:34:45:56:67",
+"Result" : "Authorized",
+"ThingList" : [
+{"Id":"0001","Type":"Door"       ,"SType":"Actuator","VType": "String","VMin" : "Open"  ,"VMax" : "Close"},
+{"Id":"0002","Type":"Light"      ,"SType":"Actuator","VType": "String","VMin" : "On"    ,"VMax" : "Off"  },
+{"Id":"0003","Type":"Presence"   ,"SType":"Sensor"  ,"VType": "String","VMin" : "AtHome","VMax" : "Away" },
+{"Id":"0004","Type":"Temperature","SType":"Sensor"  ,"VType": "Number","VMin" : "-50"   ,"VMax" : "50"   },
+{"Id":"0005","Type":"Humidity"   ,"SType":"Sensor"  ,"VType": "Number","VMin" : "0"     ,"VMax" : "100" },
+{"Id":"0006","Type":"DoorSensor" ,"SType":"Sensor"  ,"VType": "String","VMin" : "Open"  ,"VMax" : "Close"},
+{"Id":"0007","Type":"MailBox"    ,"SType":"Sensor"  ,"VType": "String","VMin" : "Empty" ,"VMax" : "Mail" },
+{"Id":"0008","Type":"Alarm"      ,"SType":"Actuator","VType": "String","VMin" : "Set"   ,"VMax" : "Unset"}
+]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +783,30 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -656,7 +880,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -692,6 +916,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -965,38 +1195,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="53.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.19921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="95.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.09765625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="53.3984375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +1242,7 @@
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
     </row>
-    <row r="2" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="34.799999999999997">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1032,10 +1262,10 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -1047,7 +1277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="132" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="139.19999999999999">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1058,31 +1288,31 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="34.799999999999997">
       <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
@@ -1093,33 +1323,33 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="69.599999999999994">
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -1128,33 +1358,33 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="87">
       <c r="B6" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -1163,33 +1393,33 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="87">
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -1201,30 +1431,30 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="121.8">
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -1233,33 +1463,33 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="87">
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -1268,33 +1498,33 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="35.4" thickBot="1">
       <c r="B10" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
@@ -1303,31 +1533,31 @@
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="34.799999999999997">
       <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1584,7 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="34.799999999999997">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1381,7 +1611,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="34.799999999999997">
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1408,7 +1638,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="34.799999999999997">
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1435,7 +1665,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="34.799999999999997">
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1462,7 +1692,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="52.2">
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1489,7 +1719,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="34.799999999999997">
       <c r="B17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1516,7 +1746,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1529,7 +1759,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1542,7 +1772,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="52.2">
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
@@ -1556,24 +1786,30 @@
         <v>53</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="J20" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="135">
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
@@ -1582,27 +1818,33 @@
         <v>52</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="J21" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="143.4">
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
@@ -1611,27 +1853,33 @@
         <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="K22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="109.8">
+      <c r="B23" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="2:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
@@ -1640,25 +1888,31 @@
         <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="J23" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1671,7 +1925,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1684,7 +1938,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12">
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
@@ -1705,7 +1959,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1718,7 +1972,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1731,7 +1985,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1744,7 +1998,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1757,7 +2011,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1770,7 +2024,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1783,7 +2037,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1796,7 +2050,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1809,7 +2063,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1822,7 +2076,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1835,7 +2089,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1848,7 +2102,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1861,7 +2115,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1874,7 +2128,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1887,7 +2141,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1900,7 +2154,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1913,7 +2167,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1926,7 +2180,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1939,7 +2193,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1952,7 +2206,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1965,7 +2219,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1978,7 +2232,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1991,7 +2245,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -2004,7 +2258,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2017,7 +2271,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2030,7 +2284,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2043,7 +2297,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -2056,7 +2310,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2069,7 +2323,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2082,7 +2336,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2095,7 +2349,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -2108,7 +2362,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -2121,7 +2375,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -2134,7 +2388,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -2147,7 +2401,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -2160,7 +2414,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -2173,7 +2427,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -2186,7 +2440,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -2199,7 +2453,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2212,7 +2466,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2225,7 +2479,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2238,7 +2492,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2251,7 +2505,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2264,7 +2518,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:12">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2277,7 +2531,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:12">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -2290,7 +2544,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:12">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -2303,7 +2557,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:12">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -2316,7 +2570,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -2329,7 +2583,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -2342,7 +2596,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -2355,7 +2609,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -2368,7 +2622,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -2381,7 +2635,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -2406,12 +2660,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TestCase for NM
update TestCase for NM
</commit_message>
<xml_diff>
--- a/doc/TestCase_0616.xlsx
+++ b/doc/TestCase_0616.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dongog.min\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16128" windowHeight="7488"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Test" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
     <author>dongog.min</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="129">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,10 +162,6 @@
     <t>TC_NM_005</t>
   </si>
   <si>
-    <t>Send action command to Link</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Input Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -188,14 +189,6 @@
     <t>TC_NM_006</t>
   </si>
   <si>
-    <t>Update current stroed things information to UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update current stroed thing information to UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Request NodeInfo from UI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,22 +213,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Send request discover to Discover</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send request register to Discover</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Updated things information from SA node</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Update changed information to RuleManager and UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC_NM_007</t>
   </si>
   <si>
@@ -244,10 +225,6 @@
   </si>
   <si>
     <t>Request removeNode from UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remove node and node's information</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -731,12 +708,73 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>"NodeID" ,"12:23:34:45:56:67"
+"ThingID", {0001~0009}
+"Value", {Open/Close}, {On/Off}, {AtHome/Away}, {number}, {number}, {Open/Close}, {Empty/Mail}, {Set/Unset}, {number}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"NodeID" ,"12:23:34:45:56:67"
+"ThingID", {0001~0009}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"NodeID" ,"12:23:34:45:56:67"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Send action command to Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Update current stroed things information to UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Update current stroed thing information to UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Send request register to Discover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Send request discover to Discover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Update changed information to RuleManager and UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Remove node and node's information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"NodeID" ,"12:23:34:45:56:67"
+"URL", "lgteam2.cc.cmu.edu"
+"Port", "550"
+"SerialNumber", "12345678"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">"ThingID", {0001~0009}
+"Type", {"Door", "Light", "Presense", "Temperature", "Humidity", DoorSensor", "MailBox", "Alarm", etc}
+"Value", {Open/Close}, {On/Off}, {AtHome/Away}, {number}, {number}, {Open/Close}, {Empty/Mail}, {Set/Unset}, {number}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,14 +952,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1195,54 +1233,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="95.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.09765625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="53.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="68.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="95.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="53.375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" ht="34.799999999999997">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1259,13 +1297,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -1277,7 +1315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="139.19999999999999">
+    <row r="3" spans="1:12" ht="132" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1288,33 +1326,33 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="34.799999999999997">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -1323,33 +1361,33 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="69.599999999999994">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -1358,33 +1396,33 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="87">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -1393,33 +1431,33 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="87">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -1431,30 +1469,30 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="121.8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -1463,33 +1501,33 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="87">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -1498,33 +1536,33 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="35.4" thickBot="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
@@ -1533,31 +1571,31 @@
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="I10" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="34.799999999999997">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="116.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1568,23 +1606,29 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="H11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="34.799999999999997">
+    <row r="12" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1595,23 +1639,29 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="H12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="34.799999999999997">
+    <row r="13" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1622,23 +1672,29 @@
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="H13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="34.799999999999997">
+    <row r="14" spans="1:12" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1649,23 +1705,29 @@
         <v>15</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="H14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="34.799999999999997">
+    <row r="15" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1676,25 +1738,31 @@
         <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="H15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="52.2">
+    <row r="16" spans="1:12" ht="182.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
@@ -1703,25 +1771,31 @@
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="H16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="2:12" ht="34.799999999999997">
+    <row r="17" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>17</v>
@@ -1730,23 +1804,29 @@
         <v>15</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="H17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1759,7 +1839,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1772,147 +1852,147 @@
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="2:12" ht="52.2">
+    <row r="20" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="K20" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="135">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="153" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>121</v>
+        <v>108</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="143.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="162.75" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="F22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="109.8">
+    </row>
+    <row r="23" spans="2:12" ht="123.75" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1925,7 +2005,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1938,7 +2018,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
@@ -1959,7 +2039,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1972,7 +2052,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1985,7 +2065,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1998,7 +2078,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2011,7 +2091,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2024,7 +2104,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -2037,7 +2117,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2050,7 +2130,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2063,7 +2143,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -2076,7 +2156,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2089,7 +2169,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2102,7 +2182,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2115,7 +2195,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2128,7 +2208,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2141,7 +2221,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2154,7 +2234,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -2167,7 +2247,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -2180,7 +2260,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="2:12">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2193,7 +2273,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="2:12">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -2206,7 +2286,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2219,7 +2299,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2232,7 +2312,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -2245,7 +2325,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -2258,7 +2338,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="2:12">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2271,7 +2351,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="2:12">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2284,7 +2364,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2297,7 +2377,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="2:12">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -2310,7 +2390,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="2:12">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2323,7 +2403,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2336,7 +2416,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2349,7 +2429,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -2362,7 +2442,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -2375,7 +2455,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -2388,7 +2468,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="2:12">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -2401,7 +2481,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="2:12">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -2414,7 +2494,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="2:12">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -2427,7 +2507,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="2:12">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -2440,7 +2520,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="2:12">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -2453,7 +2533,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2466,7 +2546,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2479,7 +2559,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="2:12">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2492,7 +2572,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2505,7 +2585,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="2:12">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2518,7 +2598,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="2:12">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2531,7 +2611,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="2:12">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -2544,7 +2624,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="2:12">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -2557,7 +2637,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="2:12">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -2570,7 +2650,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="2:12">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -2583,7 +2663,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="2:12">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -2596,7 +2676,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="2:12">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -2609,7 +2689,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="2:12">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -2622,7 +2702,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="2:12">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -2635,7 +2715,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -2660,12 +2740,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>